<commit_message>
Still setting up script
being extra careful, need to finish
</commit_message>
<xml_diff>
--- a/python/steam.xlsx
+++ b/python/steam.xlsx
@@ -67,7 +67,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -444,43 +447,96 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="1" ht="12.75" customHeight="1" s="1">
-      <c r="A1" s="2" t="inlineStr">
+    <row r="1" ht="12.75" customHeight="1" s="2">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Game</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Hours</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Hours Added Since Last</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>Last 2 Weeks Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="12.75" customHeight="1" s="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>poop</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>poop</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>poop</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="12.75" customHeight="1" s="2">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>poop</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>poop</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="12.75" customHeight="1" s="2">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>poop</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Test2</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Test3</t>
         </is>
       </c>
     </row>

</xml_diff>